<commit_message>
fix. fix unlocking failure
</commit_message>
<xml_diff>
--- a/src/main/resources/upload/flux测试.xlsx
+++ b/src/main/resources/upload/flux测试.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="17374" windowHeight="9977"/>
+    <workbookView windowWidth="17194" windowHeight="9805"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>姓名</t>
   </si>
@@ -33,11 +33,17 @@
   <si>
     <t>七七</t>
   </si>
+  <si>
+    <t>童子杰</t>
+  </si>
+  <si>
+    <t>周云挺</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
@@ -53,34 +59,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -94,14 +72,6 @@
       <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -146,6 +116,21 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -191,7 +176,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -206,49 +212,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -260,121 +350,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -397,21 +403,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -444,6 +435,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -502,148 +508,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -654,52 +660,52 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
     <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -970,13 +976,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.61261261261261" defaultRowHeight="14.1" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.61261261261261" defaultRowHeight="14.1" outlineLevelRow="4" outlineLevelCol="2"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -1008,6 +1014,28 @@
         <v>23</v>
       </c>
       <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>